<commit_message>
NP Lab RSA Algorithm
</commit_message>
<xml_diff>
--- a/software-testing-lab/8_data_driven/normal_marvel/subjects.xlsx
+++ b/software-testing-lab/8_data_driven/normal_marvel/subjects.xlsx
@@ -4,12 +4,14 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="23895" windowHeight="9975"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="15600" windowHeight="9975"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Chart2" sheetId="5" r:id="rId1"/>
+    <sheet name="Chart1" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
@@ -84,6 +86,238 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$1:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>dwn daa stm cs cn ipr sports</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="67387392"/>
+        <c:axId val="67388928"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="67387392"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="67388928"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="67388928"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="67387392"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$1:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>dwn daa stm cs cn ipr sports</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="60794752"/>
+        <c:axId val="60796288"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="60794752"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="60796288"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="60796288"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="60794752"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="78" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="78" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8670192" cy="6288942"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8670192" cy="6288942"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -373,7 +607,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>

</xml_diff>